<commit_message>
Updated: test & user defined index + column offset
</commit_message>
<xml_diff>
--- a/src/test/java/test.xlsx
+++ b/src/test/java/test.xlsx
@@ -402,14 +402,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:C7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>

</xml_diff>